<commit_message>
male izmjene nad useCaseNaplata dijagramom i scenarijom
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Naplata.xlsx
+++ b/UseCaseIScenarij/Naplata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Naziv</t>
   </si>
@@ -51,27 +51,15 @@
     <t>Naplata za događaj</t>
   </si>
   <si>
-    <t>Na osnovu događaja na koji se korisnik zeli prijaviti uposlenik obracunava iznos koji korisnik treba platiti uz mogucnost popusta za određene korisnike</t>
-  </si>
-  <si>
     <t>Korisnik zeli ici na događaj</t>
   </si>
   <si>
     <t>Korisnik mora biti registrovan na sistem, korisnik mora imati dovoljno sredstava na racunu</t>
   </si>
   <si>
-    <t>Uposlenik ima finalnu cijenu događaja o kojoj moze informisati korisnika</t>
-  </si>
-  <si>
     <t>Korisnik nema dovoljno sredstava na racunu, ne moze se prijaviti na događaj</t>
   </si>
   <si>
-    <t>Uposlenik, korisnik</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Korisnik ima uvid u listu predstojecih događaja, nakon odabira zeljenog događaja vrsi se obracun, nakon cega se stanje na racunu korisnika umanjuje za iznos racuna a stanje na racunu agencije se uvecava za isti iznos za koji je umanjeno stanje na racunu korisnika.</t>
   </si>
   <si>
@@ -90,21 +78,6 @@
     <t>1. Korisnik odabire zeljeni događaj</t>
   </si>
   <si>
-    <t>2. Uposlenik/Sistem provejrava da li korisnik ima dovoljno sredstava na racunu</t>
-  </si>
-  <si>
-    <t>3. Uposlenik/Sistem provejrava da li korisnik ima pravo na popust</t>
-  </si>
-  <si>
-    <t>4. Uposlenik/Sistem rezervise mjesto za korisnika</t>
-  </si>
-  <si>
-    <t>6. Uposlenik/Sistem uvecava stanje na racunu agencije za odgovarajuci iznos</t>
-  </si>
-  <si>
-    <t>5. Uposlenik/Sistem umanjuje stanje na racunu korinsika za odgovarajuci iznos</t>
-  </si>
-  <si>
     <t>Korisnik</t>
   </si>
   <si>
@@ -115,6 +88,30 @@
   </si>
   <si>
     <t xml:space="preserve">2. Korisnik se obavjestava da nema dovoljno sredstava na racunu </t>
+  </si>
+  <si>
+    <t>Na osnovu događaja na koji se korisnik zeli prijaviti sistem za naplatu obracunava iznos koji korisnik treba platiti uz mogucnost popusta za određene korisnike</t>
+  </si>
+  <si>
+    <t>Sistem ima finalnu cijenu događaja o kojoj moze informisati korisnika</t>
+  </si>
+  <si>
+    <t>Sistem za naplatu</t>
+  </si>
+  <si>
+    <t>2. Sistem za naplatu provejrava da li korisnik ima dovoljno sredstava na racunu</t>
+  </si>
+  <si>
+    <t>3. Sistem za naplatu provejrava da li korisnik ima pravo na popust</t>
+  </si>
+  <si>
+    <t>4. Sistem za naplatu rezervise mjesto za korisnika</t>
+  </si>
+  <si>
+    <t>5. Sistem za naplatu umanjuje stanje na racunu korinsika za odgovarajuci iznos</t>
+  </si>
+  <si>
+    <t>6. Sistem za naplatu uvecava stanje na racunu agencije za odgovarajuci iznos</t>
   </si>
 </sst>
 </file>
@@ -253,19 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border outline="0">
         <top style="medium">
@@ -276,13 +270,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B23" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B23" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:B23"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Naziv"/>
@@ -580,7 +577,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+      <selection activeCell="B23" sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -610,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1">
@@ -618,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -626,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -634,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -642,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -650,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="48.75" customHeight="1">
@@ -658,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1">
@@ -666,81 +663,81 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="12" spans="1:2">
-      <c r="A12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1"/>
     <row r="20" spans="1:2">
       <c r="A20" s="14"/>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
male izmjene nad scenarijom naplata
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Naplata.xlsx
+++ b/UseCaseIScenarij/Naplata.xlsx
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="A1:B23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>